<commit_message>
Added stages heating settings from XML file
</commit_message>
<xml_diff>
--- a/DOCs/Modbus.Table.v5.xlsx
+++ b/DOCs/Modbus.Table.v5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tranings\NTCC.NET\DOCs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{731683CD-9D97-4BAC-8A47-A2778C373802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EE92F73-8474-430C-8ED0-035112B8D9AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{25159FD2-BAFB-44FA-A08A-40EFAA6874EE}"/>
   </bookViews>
@@ -2101,33 +2101,18 @@
     <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="16">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Roboto Condensed Light"/>
-        <charset val="204"/>
-        <scheme val="none"/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -2375,6 +2360,21 @@
         <vertAlign val="baseline"/>
         <sz val="12"/>
         <color theme="1"/>
+        <name val="Roboto Condensed Light"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
         <name val="Roboto Condensed"/>
         <charset val="204"/>
         <scheme val="none"/>
@@ -2439,46 +2439,69 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{67812D53-6DA3-4072-8486-4FC97F40BD52}" name="Таблица13" displayName="Таблица13" ref="A1:M208" tableType="xml" totalsRowShown="0" headerRowDxfId="15" dataDxfId="0" tableBorderDxfId="14">
-  <autoFilter ref="A1:M208" xr:uid="{67812D53-6DA3-4072-8486-4FC97F40BD52}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{67812D53-6DA3-4072-8486-4FC97F40BD52}" name="Таблица13" displayName="Таблица13" ref="A1:M208" tableType="xml" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" tableBorderDxfId="13">
+  <autoFilter ref="A1:M208" xr:uid="{67812D53-6DA3-4072-8486-4FC97F40BD52}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="AO"/>
+        <filter val="DO"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="2">
+      <filters>
+        <filter val="КЛАПАН"/>
+        <filter val="КОНТРОЛЬ СВЯЗИ"/>
+        <filter val="ОХЛАЖДЕНИЕ"/>
+        <filter val="РАСХОДОМЕР BRONKHORST"/>
+        <filter val="РАСХОДОМЕР MD400C"/>
+        <filter val="СИГНАЛ HT01"/>
+        <filter val="СИГНАЛ HT02"/>
+        <filter val="СИГНАЛ HT03"/>
+        <filter val="СИГНАЛ HT04"/>
+        <filter val="СИГНАЛ HT05"/>
+        <filter val="СИГНАЛ HT06"/>
+        <filter val="СИГНАЛ HT07"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="13">
-    <tableColumn id="7" xr3:uid="{F344DDFE-4630-4BDE-8A8B-635BC9E0DF04}" uniqueName="Type" name="Type" dataDxfId="13">
+    <tableColumn id="7" xr3:uid="{F344DDFE-4630-4BDE-8A8B-635BC9E0DF04}" uniqueName="Type" name="Type" dataDxfId="12">
       <xmlColumnPr mapId="1" xpath="/DataPoints/DataPoint/@Type" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{E2B6C207-400B-4E1C-AC34-59FF08073289}" uniqueName="ID" name="ID" dataDxfId="12">
+    <tableColumn id="2" xr3:uid="{E2B6C207-400B-4E1C-AC34-59FF08073289}" uniqueName="ID" name="ID" dataDxfId="11">
       <xmlColumnPr mapId="1" xpath="/DataPoints/DataPoint/@ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{2E615F97-0114-4DC8-811B-F44C39D87BE3}" uniqueName="Name" name="Name" dataDxfId="11">
+    <tableColumn id="3" xr3:uid="{2E615F97-0114-4DC8-811B-F44C39D87BE3}" uniqueName="Name" name="Name" dataDxfId="10">
       <xmlColumnPr mapId="1" xpath="/DataPoints/DataPoint/@Name" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{77A1C40E-F02C-41A8-8F8C-2166E935A189}" uniqueName="DeviceID" name="DeviceID" dataDxfId="10">
+    <tableColumn id="4" xr3:uid="{77A1C40E-F02C-41A8-8F8C-2166E935A189}" uniqueName="DeviceID" name="DeviceID" dataDxfId="9">
       <xmlColumnPr mapId="1" xpath="/DataPoints/DataPoint/@DeviceID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{7B477474-A41C-44D8-94E3-3DF99120638C}" uniqueName="Group" name="Group" dataDxfId="9">
+    <tableColumn id="10" xr3:uid="{7B477474-A41C-44D8-94E3-3DF99120638C}" uniqueName="Group" name="Group" dataDxfId="8">
       <xmlColumnPr mapId="1" xpath="/DataPoints/DataPoint/@Group" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{D15AEE10-426C-4B92-A46E-DD90A7E75024}" uniqueName="Channel" name="Channel" dataDxfId="8">
+    <tableColumn id="8" xr3:uid="{D15AEE10-426C-4B92-A46E-DD90A7E75024}" uniqueName="Channel" name="Channel" dataDxfId="7">
       <xmlColumnPr mapId="1" xpath="/DataPoints/DataPoint/@Channel" xmlDataType="unsignedByte"/>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{706FB1FD-2943-40F3-BF0D-8EF27C45617A}" uniqueName="ToStr" name="ToStr" dataDxfId="7">
+    <tableColumn id="5" xr3:uid="{706FB1FD-2943-40F3-BF0D-8EF27C45617A}" uniqueName="ToStr" name="ToStr" dataDxfId="6">
       <xmlColumnPr mapId="1" xpath="/DataPoints/DataPoint/@ToStr" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{792F88C6-9769-4024-BA7E-9D914D4FB0E3}" uniqueName="MinSignal" name="MinSignal" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{792F88C6-9769-4024-BA7E-9D914D4FB0E3}" uniqueName="MinSignal" name="MinSignal" dataDxfId="5">
       <xmlColumnPr mapId="1" xpath="/DataPoints/DataPoint/@MinSignal" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{5A5D2E76-B4B1-4661-838B-D2505901359B}" uniqueName="MaxSignal" name="MaxSignal" dataDxfId="5">
+    <tableColumn id="9" xr3:uid="{5A5D2E76-B4B1-4661-838B-D2505901359B}" uniqueName="MaxSignal" name="MaxSignal" dataDxfId="4">
       <xmlColumnPr mapId="1" xpath="/DataPoints/DataPoint/@MaxSignal" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{9395F739-A420-43DC-8DB8-1723AD4AB7E6}" uniqueName="MinValue" name="MinValue" dataDxfId="4">
+    <tableColumn id="12" xr3:uid="{9395F739-A420-43DC-8DB8-1723AD4AB7E6}" uniqueName="MinValue" name="MinValue" dataDxfId="3">
       <xmlColumnPr mapId="1" xpath="/DataPoints/DataPoint/@MinValue" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{A48AA711-D247-4851-8BC5-CDB046B40691}" uniqueName="MaxValue" name="МахValue" dataDxfId="3">
+    <tableColumn id="11" xr3:uid="{A48AA711-D247-4851-8BC5-CDB046B40691}" uniqueName="MaxValue" name="МахValue" dataDxfId="2">
       <xmlColumnPr mapId="1" xpath="/DataPoints/DataPoint/@MaxValue" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{3AEDC1E2-0F83-4FE8-A22A-377F89D11B21}" uniqueName="Units" name="Units" dataDxfId="2">
+    <tableColumn id="13" xr3:uid="{3AEDC1E2-0F83-4FE8-A22A-377F89D11B21}" uniqueName="Units" name="Units" dataDxfId="1">
       <xmlColumnPr mapId="1" xpath="/DataPoints/DataPoint/@Units" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{9D123D3A-6D7B-4792-959C-1E09E63EA497}" uniqueName="DataPoint" name="Description" dataDxfId="1">
+    <tableColumn id="6" xr3:uid="{9D123D3A-6D7B-4792-959C-1E09E63EA497}" uniqueName="DataPoint" name="Description" dataDxfId="0">
       <xmlColumnPr mapId="1" xpath="/DataPoints/DataPoint" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -2801,14 +2824,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>151</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
       <c r="H1" s="15" t="s">
         <v>235</v>
       </c>
@@ -2834,14 +2857,14 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="35" t="s">
         <v>152</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
@@ -3655,14 +3678,14 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="34" t="s">
+      <c r="A43" s="35" t="s">
         <v>154</v>
       </c>
-      <c r="B43" s="34"/>
-      <c r="C43" s="34"/>
-      <c r="D43" s="34"/>
-      <c r="E43" s="34"/>
-      <c r="F43" s="34"/>
+      <c r="B43" s="35"/>
+      <c r="C43" s="35"/>
+      <c r="D43" s="35"/>
+      <c r="E43" s="35"/>
+      <c r="F43" s="35"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
@@ -4877,14 +4900,14 @@
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A104" s="34" t="s">
+      <c r="A104" s="35" t="s">
         <v>155</v>
       </c>
-      <c r="B104" s="34"/>
-      <c r="C104" s="34"/>
-      <c r="D104" s="34"/>
-      <c r="E104" s="34"/>
-      <c r="F104" s="34"/>
+      <c r="B104" s="35"/>
+      <c r="C104" s="35"/>
+      <c r="D104" s="35"/>
+      <c r="E104" s="35"/>
+      <c r="F104" s="35"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" s="2">
@@ -5207,14 +5230,14 @@
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A121" s="34" t="s">
+      <c r="A121" s="35" t="s">
         <v>156</v>
       </c>
-      <c r="B121" s="34"/>
-      <c r="C121" s="34"/>
-      <c r="D121" s="34"/>
-      <c r="E121" s="34"/>
-      <c r="F121" s="34"/>
+      <c r="B121" s="35"/>
+      <c r="C121" s="35"/>
+      <c r="D121" s="35"/>
+      <c r="E121" s="35"/>
+      <c r="F121" s="35"/>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122" s="2">
@@ -5697,14 +5720,14 @@
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A146" s="34" t="s">
+      <c r="A146" s="35" t="s">
         <v>281</v>
       </c>
-      <c r="B146" s="34"/>
-      <c r="C146" s="34"/>
-      <c r="D146" s="34"/>
-      <c r="E146" s="34"/>
-      <c r="F146" s="34"/>
+      <c r="B146" s="35"/>
+      <c r="C146" s="35"/>
+      <c r="D146" s="35"/>
+      <c r="E146" s="35"/>
+      <c r="F146" s="35"/>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147" s="2">
@@ -5847,14 +5870,14 @@
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A154" s="34" t="s">
+      <c r="A154" s="35" t="s">
         <v>282</v>
       </c>
-      <c r="B154" s="34"/>
-      <c r="C154" s="34"/>
-      <c r="D154" s="34"/>
-      <c r="E154" s="34"/>
-      <c r="F154" s="34"/>
+      <c r="B154" s="35"/>
+      <c r="C154" s="35"/>
+      <c r="D154" s="35"/>
+      <c r="E154" s="35"/>
+      <c r="F154" s="35"/>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A155" s="2">
@@ -5997,14 +6020,14 @@
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A162" s="34" t="s">
+      <c r="A162" s="35" t="s">
         <v>283</v>
       </c>
-      <c r="B162" s="34"/>
-      <c r="C162" s="34"/>
-      <c r="D162" s="34"/>
-      <c r="E162" s="34"/>
-      <c r="F162" s="34"/>
+      <c r="B162" s="35"/>
+      <c r="C162" s="35"/>
+      <c r="D162" s="35"/>
+      <c r="E162" s="35"/>
+      <c r="F162" s="35"/>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A163" s="2">
@@ -6147,14 +6170,14 @@
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A170" s="34" t="s">
+      <c r="A170" s="35" t="s">
         <v>284</v>
       </c>
-      <c r="B170" s="34"/>
-      <c r="C170" s="34"/>
-      <c r="D170" s="34"/>
-      <c r="E170" s="34"/>
-      <c r="F170" s="34"/>
+      <c r="B170" s="35"/>
+      <c r="C170" s="35"/>
+      <c r="D170" s="35"/>
+      <c r="E170" s="35"/>
+      <c r="F170" s="35"/>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A171" s="2">
@@ -6297,14 +6320,14 @@
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A178" s="34" t="s">
+      <c r="A178" s="35" t="s">
         <v>285</v>
       </c>
-      <c r="B178" s="34"/>
-      <c r="C178" s="34"/>
-      <c r="D178" s="34"/>
-      <c r="E178" s="34"/>
-      <c r="F178" s="34"/>
+      <c r="B178" s="35"/>
+      <c r="C178" s="35"/>
+      <c r="D178" s="35"/>
+      <c r="E178" s="35"/>
+      <c r="F178" s="35"/>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A179" s="2">
@@ -6447,14 +6470,14 @@
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A186" s="34" t="s">
+      <c r="A186" s="35" t="s">
         <v>287</v>
       </c>
-      <c r="B186" s="34"/>
-      <c r="C186" s="34"/>
-      <c r="D186" s="34"/>
-      <c r="E186" s="34"/>
-      <c r="F186" s="34"/>
+      <c r="B186" s="35"/>
+      <c r="C186" s="35"/>
+      <c r="D186" s="35"/>
+      <c r="E186" s="35"/>
+      <c r="F186" s="35"/>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A187" s="2">
@@ -6597,14 +6620,14 @@
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A194" s="34" t="s">
+      <c r="A194" s="35" t="s">
         <v>286</v>
       </c>
-      <c r="B194" s="34"/>
-      <c r="C194" s="34"/>
-      <c r="D194" s="34"/>
-      <c r="E194" s="34"/>
-      <c r="F194" s="34"/>
+      <c r="B194" s="35"/>
+      <c r="C194" s="35"/>
+      <c r="D194" s="35"/>
+      <c r="E194" s="35"/>
+      <c r="F194" s="35"/>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A195" s="2">
@@ -6747,14 +6770,14 @@
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A202" s="34" t="s">
+      <c r="A202" s="35" t="s">
         <v>293</v>
       </c>
-      <c r="B202" s="34"/>
-      <c r="C202" s="34"/>
-      <c r="D202" s="34"/>
-      <c r="E202" s="34"/>
-      <c r="F202" s="34"/>
+      <c r="B202" s="35"/>
+      <c r="C202" s="35"/>
+      <c r="D202" s="35"/>
+      <c r="E202" s="35"/>
+      <c r="F202" s="35"/>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A203" s="2">
@@ -6817,14 +6840,14 @@
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A206" s="34" t="s">
+      <c r="A206" s="35" t="s">
         <v>297</v>
       </c>
-      <c r="B206" s="34"/>
-      <c r="C206" s="34"/>
-      <c r="D206" s="34"/>
-      <c r="E206" s="34"/>
-      <c r="F206" s="34"/>
+      <c r="B206" s="35"/>
+      <c r="C206" s="35"/>
+      <c r="D206" s="35"/>
+      <c r="E206" s="35"/>
+      <c r="F206" s="35"/>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A207" s="2">
@@ -6887,14 +6910,14 @@
       </c>
     </row>
     <row r="210" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A210" s="34" t="s">
+      <c r="A210" s="35" t="s">
         <v>298</v>
       </c>
-      <c r="B210" s="34"/>
-      <c r="C210" s="34"/>
-      <c r="D210" s="34"/>
-      <c r="E210" s="34"/>
-      <c r="F210" s="34"/>
+      <c r="B210" s="35"/>
+      <c r="C210" s="35"/>
+      <c r="D210" s="35"/>
+      <c r="E210" s="35"/>
+      <c r="F210" s="35"/>
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A211" s="2">
@@ -6957,14 +6980,14 @@
       </c>
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A214" s="34" t="s">
+      <c r="A214" s="35" t="s">
         <v>294</v>
       </c>
-      <c r="B214" s="34"/>
-      <c r="C214" s="34"/>
-      <c r="D214" s="34"/>
-      <c r="E214" s="34"/>
-      <c r="F214" s="34"/>
+      <c r="B214" s="35"/>
+      <c r="C214" s="35"/>
+      <c r="D214" s="35"/>
+      <c r="E214" s="35"/>
+      <c r="F214" s="35"/>
       <c r="H214" s="18" t="s">
         <v>295</v>
       </c>
@@ -7030,14 +7053,14 @@
       </c>
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A218" s="34" t="s">
+      <c r="A218" s="35" t="s">
         <v>164</v>
       </c>
-      <c r="B218" s="34"/>
-      <c r="C218" s="34"/>
-      <c r="D218" s="34"/>
-      <c r="E218" s="34"/>
-      <c r="F218" s="34"/>
+      <c r="B218" s="35"/>
+      <c r="C218" s="35"/>
+      <c r="D218" s="35"/>
+      <c r="E218" s="35"/>
+      <c r="F218" s="35"/>
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A219" s="2">
@@ -7100,14 +7123,14 @@
       </c>
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A222" s="34" t="s">
+      <c r="A222" s="35" t="s">
         <v>165</v>
       </c>
-      <c r="B222" s="34"/>
-      <c r="C222" s="34"/>
-      <c r="D222" s="34"/>
-      <c r="E222" s="34"/>
-      <c r="F222" s="34"/>
+      <c r="B222" s="35"/>
+      <c r="C222" s="35"/>
+      <c r="D222" s="35"/>
+      <c r="E222" s="35"/>
+      <c r="F222" s="35"/>
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A223" s="2">
@@ -7190,14 +7213,14 @@
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A227" s="34" t="s">
+      <c r="A227" s="35" t="s">
         <v>238</v>
       </c>
-      <c r="B227" s="34"/>
-      <c r="C227" s="34"/>
-      <c r="D227" s="34"/>
-      <c r="E227" s="34"/>
-      <c r="F227" s="34"/>
+      <c r="B227" s="35"/>
+      <c r="C227" s="35"/>
+      <c r="D227" s="35"/>
+      <c r="E227" s="35"/>
+      <c r="F227" s="35"/>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A228" s="2">
@@ -7221,6 +7244,18 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A206:F206"/>
+    <mergeCell ref="A210:F210"/>
+    <mergeCell ref="A214:F214"/>
+    <mergeCell ref="A227:F227"/>
+    <mergeCell ref="A222:F222"/>
+    <mergeCell ref="A218:F218"/>
+    <mergeCell ref="A146:F146"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A43:F43"/>
+    <mergeCell ref="A104:F104"/>
+    <mergeCell ref="A121:F121"/>
     <mergeCell ref="A194:F194"/>
     <mergeCell ref="A202:F202"/>
     <mergeCell ref="A154:F154"/>
@@ -7228,18 +7263,6 @@
     <mergeCell ref="A170:F170"/>
     <mergeCell ref="A178:F178"/>
     <mergeCell ref="A186:F186"/>
-    <mergeCell ref="A146:F146"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A43:F43"/>
-    <mergeCell ref="A104:F104"/>
-    <mergeCell ref="A121:F121"/>
-    <mergeCell ref="A206:F206"/>
-    <mergeCell ref="A210:F210"/>
-    <mergeCell ref="A214:F214"/>
-    <mergeCell ref="A227:F227"/>
-    <mergeCell ref="A222:F222"/>
-    <mergeCell ref="A218:F218"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7251,8 +7274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C160DD2-CD62-4538-812B-8C6818687863}">
   <dimension ref="A1:M208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A194" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F209" sqref="F209"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7308,7 +7331,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="26" t="s">
         <v>317</v>
       </c>
@@ -7337,7 +7360,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>317</v>
       </c>
@@ -7366,7 +7389,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
         <v>317</v>
       </c>
@@ -7395,7 +7418,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="26" t="s">
         <v>317</v>
       </c>
@@ -7424,7 +7447,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="26" t="s">
         <v>317</v>
       </c>
@@ -7453,7 +7476,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
         <v>317</v>
       </c>
@@ -7482,7 +7505,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="26" t="s">
         <v>317</v>
       </c>
@@ -7511,7 +7534,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="26" t="s">
         <v>317</v>
       </c>
@@ -7540,7 +7563,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="26" t="s">
         <v>317</v>
       </c>
@@ -7569,7 +7592,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="26" t="s">
         <v>317</v>
       </c>
@@ -7598,7 +7621,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="26" t="s">
         <v>317</v>
       </c>
@@ -7627,7 +7650,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="26" t="s">
         <v>317</v>
       </c>
@@ -7656,7 +7679,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="26" t="s">
         <v>317</v>
       </c>
@@ -7685,7 +7708,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="26" t="s">
         <v>317</v>
       </c>
@@ -7714,7 +7737,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="26" t="s">
         <v>317</v>
       </c>
@@ -7743,7 +7766,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="26" t="s">
         <v>317</v>
       </c>
@@ -7772,7 +7795,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="26" t="s">
         <v>317</v>
       </c>
@@ -7801,7 +7824,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="26" t="s">
         <v>317</v>
       </c>
@@ -7830,7 +7853,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="26" t="s">
         <v>317</v>
       </c>
@@ -7859,7 +7882,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="26" t="s">
         <v>317</v>
       </c>
@@ -7888,7 +7911,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="26" t="s">
         <v>317</v>
       </c>
@@ -7917,7 +7940,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="26" t="s">
         <v>317</v>
       </c>
@@ -7946,7 +7969,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="26" t="s">
         <v>317</v>
       </c>
@@ -7975,7 +7998,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="26" t="s">
         <v>317</v>
       </c>
@@ -8004,7 +8027,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="26" t="s">
         <v>317</v>
       </c>
@@ -8033,7 +8056,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="26" t="s">
         <v>317</v>
       </c>
@@ -8062,7 +8085,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="26" t="s">
         <v>317</v>
       </c>
@@ -8091,7 +8114,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="26" t="s">
         <v>317</v>
       </c>
@@ -8120,7 +8143,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="26" t="s">
         <v>317</v>
       </c>
@@ -8149,7 +8172,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="26" t="s">
         <v>317</v>
       </c>
@@ -8178,7 +8201,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="26" t="s">
         <v>317</v>
       </c>
@@ -8207,7 +8230,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="26" t="s">
         <v>317</v>
       </c>
@@ -8236,7 +8259,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="26" t="s">
         <v>317</v>
       </c>
@@ -8265,7 +8288,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="26" t="s">
         <v>317</v>
       </c>
@@ -8294,7 +8317,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="26" t="s">
         <v>317</v>
       </c>
@@ -8323,7 +8346,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="26" t="s">
         <v>317</v>
       </c>
@@ -8352,7 +8375,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="26" t="s">
         <v>317</v>
       </c>
@@ -8381,7 +8404,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="26" t="s">
         <v>317</v>
       </c>
@@ -8410,7 +8433,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="26" t="s">
         <v>365</v>
       </c>
@@ -8439,7 +8462,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="26" t="s">
         <v>365</v>
       </c>
@@ -8468,7 +8491,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="26" t="s">
         <v>365</v>
       </c>
@@ -8497,7 +8520,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="26" t="s">
         <v>365</v>
       </c>
@@ -8526,7 +8549,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="26" t="s">
         <v>365</v>
       </c>
@@ -8555,7 +8578,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="45" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="26" t="s">
         <v>365</v>
       </c>
@@ -8584,7 +8607,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="46" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="26" t="s">
         <v>365</v>
       </c>
@@ -8613,7 +8636,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="47" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="26" t="s">
         <v>365</v>
       </c>
@@ -8642,7 +8665,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="48" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="26" t="s">
         <v>365</v>
       </c>
@@ -8671,7 +8694,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="49" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="26" t="s">
         <v>365</v>
       </c>
@@ -8729,7 +8752,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="51" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="26" t="s">
         <v>365</v>
       </c>
@@ -8758,7 +8781,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="52" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="26" t="s">
         <v>365</v>
       </c>
@@ -8787,7 +8810,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="53" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="26" t="s">
         <v>365</v>
       </c>
@@ -8816,7 +8839,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="54" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="26" t="s">
         <v>365</v>
       </c>
@@ -8845,7 +8868,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="55" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="26" t="s">
         <v>365</v>
       </c>
@@ -8874,7 +8897,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="56" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="26" t="s">
         <v>365</v>
       </c>
@@ -8903,7 +8926,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="57" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="26" t="s">
         <v>365</v>
       </c>
@@ -8932,7 +8955,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="58" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="26" t="s">
         <v>365</v>
       </c>
@@ -8961,7 +8984,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="59" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="26" t="s">
         <v>365</v>
       </c>
@@ -8990,7 +9013,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="60" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="26" t="s">
         <v>365</v>
       </c>
@@ -9019,7 +9042,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="61" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="26" t="s">
         <v>365</v>
       </c>
@@ -9048,7 +9071,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="62" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="26" t="s">
         <v>365</v>
       </c>
@@ -9077,7 +9100,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="63" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="26" t="s">
         <v>365</v>
       </c>
@@ -9106,7 +9129,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="64" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="26" t="s">
         <v>365</v>
       </c>
@@ -9135,7 +9158,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="65" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="26" t="s">
         <v>365</v>
       </c>
@@ -9164,7 +9187,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="66" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="26" t="s">
         <v>365</v>
       </c>
@@ -9193,7 +9216,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="67" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="26" t="s">
         <v>365</v>
       </c>
@@ -9222,7 +9245,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="68" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="26" t="s">
         <v>365</v>
       </c>
@@ -9251,7 +9274,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="69" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="26" t="s">
         <v>365</v>
       </c>
@@ -9280,7 +9303,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="70" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="26" t="s">
         <v>365</v>
       </c>
@@ -9309,7 +9332,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="71" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="26" t="s">
         <v>365</v>
       </c>
@@ -9338,7 +9361,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="72" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="26" t="s">
         <v>365</v>
       </c>
@@ -9367,7 +9390,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="73" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="26" t="s">
         <v>365</v>
       </c>
@@ -9396,7 +9419,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="74" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="26" t="s">
         <v>365</v>
       </c>
@@ -9425,7 +9448,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="75" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="26" t="s">
         <v>365</v>
       </c>
@@ -9947,7 +9970,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="93" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="26" t="s">
         <v>365</v>
       </c>
@@ -9976,7 +9999,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="94" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="26" t="s">
         <v>365</v>
       </c>
@@ -10005,7 +10028,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="95" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="26" t="s">
         <v>365</v>
       </c>
@@ -10034,7 +10057,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="96" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="26" t="s">
         <v>365</v>
       </c>
@@ -10063,7 +10086,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="97" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="26" t="s">
         <v>365</v>
       </c>
@@ -10092,7 +10115,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="98" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="26" t="s">
         <v>365</v>
       </c>
@@ -10121,7 +10144,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="99" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="26" t="s">
         <v>365</v>
       </c>
@@ -10150,7 +10173,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="100" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="26" t="s">
         <v>438</v>
       </c>
@@ -10191,7 +10214,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="101" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="26" t="s">
         <v>438</v>
       </c>
@@ -10232,7 +10255,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="102" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="26" t="s">
         <v>438</v>
       </c>
@@ -10273,7 +10296,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="103" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="26" t="s">
         <v>438</v>
       </c>
@@ -10314,7 +10337,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="104" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="26" t="s">
         <v>438</v>
       </c>
@@ -10355,7 +10378,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="105" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="26" t="s">
         <v>438</v>
       </c>
@@ -10396,7 +10419,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="106" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="26" t="s">
         <v>438</v>
       </c>
@@ -10437,7 +10460,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="107" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="26" t="s">
         <v>438</v>
       </c>
@@ -10478,7 +10501,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="108" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="26" t="s">
         <v>438</v>
       </c>
@@ -10519,7 +10542,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="109" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="26" t="s">
         <v>438</v>
       </c>
@@ -10558,7 +10581,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="110" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="26" t="s">
         <v>438</v>
       </c>
@@ -10599,7 +10622,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="111" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="26" t="s">
         <v>438</v>
       </c>
@@ -10640,7 +10663,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="112" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="26" t="s">
         <v>438</v>
       </c>
@@ -10681,7 +10704,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="113" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="26" t="s">
         <v>438</v>
       </c>
@@ -10722,7 +10745,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="114" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="26" t="s">
         <v>438</v>
       </c>
@@ -10763,7 +10786,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="115" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="26" t="s">
         <v>438</v>
       </c>
@@ -10802,7 +10825,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="116" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="26" t="s">
         <v>438</v>
       </c>
@@ -10843,7 +10866,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="117" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="26" t="s">
         <v>438</v>
       </c>
@@ -10884,7 +10907,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="118" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="26" t="s">
         <v>438</v>
       </c>
@@ -10925,7 +10948,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="119" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="26" t="s">
         <v>438</v>
       </c>
@@ -10966,7 +10989,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="120" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="26" t="s">
         <v>438</v>
       </c>
@@ -11007,7 +11030,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="121" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="26" t="s">
         <v>438</v>
       </c>
@@ -11048,7 +11071,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="122" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="26" t="s">
         <v>438</v>
       </c>
@@ -11089,7 +11112,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="123" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="26" t="s">
         <v>438</v>
       </c>
@@ -11130,7 +11153,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="124" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="26" t="s">
         <v>438</v>
       </c>
@@ -11171,7 +11194,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="125" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="26" t="s">
         <v>438</v>
       </c>
@@ -11212,7 +11235,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="126" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="26" t="s">
         <v>438</v>
       </c>
@@ -11253,7 +11276,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="127" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="26" t="s">
         <v>438</v>
       </c>
@@ -11294,7 +11317,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="128" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="26" t="s">
         <v>438</v>
       </c>
@@ -11335,7 +11358,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="129" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="26" t="s">
         <v>438</v>
       </c>
@@ -11376,7 +11399,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="130" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="26" t="s">
         <v>438</v>
       </c>
@@ -11417,7 +11440,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="131" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="26" t="s">
         <v>438</v>
       </c>
@@ -11458,7 +11481,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="132" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="26" t="s">
         <v>438</v>
       </c>
@@ -11499,7 +11522,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="133" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="26" t="s">
         <v>438</v>
       </c>
@@ -11540,7 +11563,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="134" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="26" t="s">
         <v>438</v>
       </c>
@@ -11581,7 +11604,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="135" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="26" t="s">
         <v>438</v>
       </c>
@@ -11622,7 +11645,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="136" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="26" t="s">
         <v>438</v>
       </c>
@@ -11663,7 +11686,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="137" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="26" t="s">
         <v>438</v>
       </c>
@@ -11692,7 +11715,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="138" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="26" t="s">
         <v>438</v>
       </c>
@@ -11721,7 +11744,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="139" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="26" t="s">
         <v>438</v>
       </c>
@@ -11750,7 +11773,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="140" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="26" t="s">
         <v>438</v>
       </c>
@@ -11791,7 +11814,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="141" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="26" t="s">
         <v>438</v>
       </c>
@@ -11832,7 +11855,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="142" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="26" t="s">
         <v>438</v>
       </c>
@@ -11871,7 +11894,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="143" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="26" t="s">
         <v>317</v>
       </c>
@@ -11900,7 +11923,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="144" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="26" t="s">
         <v>317</v>
       </c>
@@ -11987,7 +12010,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="147" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="26" t="s">
         <v>438</v>
       </c>
@@ -12028,7 +12051,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="148" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="26" t="s">
         <v>438</v>
       </c>
@@ -12069,7 +12092,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="149" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="26" t="s">
         <v>438</v>
       </c>
@@ -12108,7 +12131,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="150" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="26" t="s">
         <v>317</v>
       </c>
@@ -12137,7 +12160,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="151" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="26" t="s">
         <v>317</v>
       </c>
@@ -12248,7 +12271,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="154" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="26" t="s">
         <v>438</v>
       </c>
@@ -12289,7 +12312,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="155" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" s="26" t="s">
         <v>438</v>
       </c>
@@ -12330,7 +12353,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="156" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="26" t="s">
         <v>438</v>
       </c>
@@ -12369,7 +12392,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="157" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="26" t="s">
         <v>317</v>
       </c>
@@ -12398,7 +12421,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="158" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="26" t="s">
         <v>317</v>
       </c>
@@ -12509,7 +12532,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="161" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" s="26" t="s">
         <v>438</v>
       </c>
@@ -12550,7 +12573,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="162" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="26" t="s">
         <v>438</v>
       </c>
@@ -12591,7 +12614,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="163" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" s="26" t="s">
         <v>438</v>
       </c>
@@ -12630,7 +12653,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="164" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164" s="26" t="s">
         <v>317</v>
       </c>
@@ -12659,7 +12682,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="165" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" s="26" t="s">
         <v>317</v>
       </c>
@@ -12770,7 +12793,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="168" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168" s="26" t="s">
         <v>438</v>
       </c>
@@ -12811,7 +12834,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="169" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169" s="26" t="s">
         <v>438</v>
       </c>
@@ -12852,7 +12875,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="170" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170" s="26" t="s">
         <v>438</v>
       </c>
@@ -12891,7 +12914,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="171" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" s="26" t="s">
         <v>317</v>
       </c>
@@ -12920,7 +12943,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="172" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" s="26" t="s">
         <v>317</v>
       </c>
@@ -13031,7 +13054,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="175" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" s="26" t="s">
         <v>438</v>
       </c>
@@ -13072,7 +13095,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="176" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176" s="26" t="s">
         <v>438</v>
       </c>
@@ -13113,7 +13136,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="177" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177" s="26" t="s">
         <v>438</v>
       </c>
@@ -13152,7 +13175,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="178" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A178" s="26" t="s">
         <v>317</v>
       </c>
@@ -13181,7 +13204,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="179" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A179" s="26" t="s">
         <v>317</v>
       </c>
@@ -13292,7 +13315,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="182" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A182" s="26" t="s">
         <v>438</v>
       </c>
@@ -13333,7 +13356,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="183" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A183" s="26" t="s">
         <v>438</v>
       </c>
@@ -13374,7 +13397,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="184" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A184" s="26" t="s">
         <v>438</v>
       </c>
@@ -13413,7 +13436,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="185" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A185" s="26" t="s">
         <v>317</v>
       </c>
@@ -13442,7 +13465,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="186" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A186" s="26" t="s">
         <v>317</v>
       </c>
@@ -13553,7 +13576,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="189" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A189" s="26" t="s">
         <v>438</v>
       </c>
@@ -13590,11 +13613,11 @@
       <c r="L189" s="26" t="s">
         <v>591</v>
       </c>
-      <c r="M189" s="36" t="s">
+      <c r="M189" s="34" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="190" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A190" s="26" t="s">
         <v>438</v>
       </c>
@@ -13631,11 +13654,11 @@
       <c r="L190" s="26" t="s">
         <v>591</v>
       </c>
-      <c r="M190" s="36" t="s">
+      <c r="M190" s="34" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="191" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A191" s="26" t="s">
         <v>438</v>
       </c>
@@ -13660,11 +13683,11 @@
       <c r="J191" s="26"/>
       <c r="K191" s="26"/>
       <c r="L191" s="26"/>
-      <c r="M191" s="36" t="s">
+      <c r="M191" s="34" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="192" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A192" s="26" t="s">
         <v>438</v>
       </c>
@@ -13701,11 +13724,11 @@
       <c r="L192" s="26" t="s">
         <v>591</v>
       </c>
-      <c r="M192" s="36" t="s">
+      <c r="M192" s="34" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="193" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A193" s="26" t="s">
         <v>438</v>
       </c>
@@ -13742,11 +13765,11 @@
       <c r="L193" s="26" t="s">
         <v>591</v>
       </c>
-      <c r="M193" s="36" t="s">
+      <c r="M193" s="34" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="194" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A194" s="26" t="s">
         <v>438</v>
       </c>
@@ -13771,11 +13794,11 @@
       <c r="J194" s="26"/>
       <c r="K194" s="26"/>
       <c r="L194" s="26"/>
-      <c r="M194" s="36" t="s">
+      <c r="M194" s="34" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="195" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A195" s="26" t="s">
         <v>438</v>
       </c>
@@ -13812,11 +13835,11 @@
       <c r="L195" s="26" t="s">
         <v>591</v>
       </c>
-      <c r="M195" s="36" t="s">
+      <c r="M195" s="34" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="196" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A196" s="26" t="s">
         <v>438</v>
       </c>
@@ -13853,11 +13876,11 @@
       <c r="L196" s="26" t="s">
         <v>591</v>
       </c>
-      <c r="M196" s="36" t="s">
+      <c r="M196" s="34" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="197" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A197" s="26" t="s">
         <v>438</v>
       </c>
@@ -13882,11 +13905,11 @@
       <c r="J197" s="26"/>
       <c r="K197" s="26"/>
       <c r="L197" s="26"/>
-      <c r="M197" s="36" t="s">
+      <c r="M197" s="34" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="198" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A198" s="26" t="s">
         <v>438</v>
       </c>
@@ -13923,11 +13946,11 @@
       <c r="L198" s="26" t="s">
         <v>591</v>
       </c>
-      <c r="M198" s="36" t="s">
+      <c r="M198" s="34" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="199" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A199" s="26" t="s">
         <v>438</v>
       </c>
@@ -13964,11 +13987,11 @@
       <c r="L199" s="26" t="s">
         <v>591</v>
       </c>
-      <c r="M199" s="36" t="s">
+      <c r="M199" s="34" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="200" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A200" s="26" t="s">
         <v>438</v>
       </c>
@@ -13993,11 +14016,11 @@
       <c r="J200" s="26"/>
       <c r="K200" s="26"/>
       <c r="L200" s="26"/>
-      <c r="M200" s="36" t="s">
+      <c r="M200" s="34" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="201" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A201" s="26" t="s">
         <v>438</v>
       </c>
@@ -14038,7 +14061,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="202" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A202" s="26" t="s">
         <v>438</v>
       </c>
@@ -14112,7 +14135,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="204" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A204" s="26" t="s">
         <v>438</v>
       </c>
@@ -14153,7 +14176,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="205" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A205" s="26" t="s">
         <v>438</v>
       </c>
@@ -14194,7 +14217,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="206" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:13" s="31" customFormat="1" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A206" s="26" t="s">
         <v>438</v>
       </c>

</xml_diff>

<commit_message>
Added interface for automatic mode - added stages tracking control - added schema for heands control and auto mode checking - added popup stage events notifications
</commit_message>
<xml_diff>
--- a/DOCs/Modbus.Table.v5.xlsx
+++ b/DOCs/Modbus.Table.v5.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tranings\NTCC.NET\DOCs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{953DAFDF-FEB4-47A1-8377-971920684141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD476EA-3075-4DB7-AC95-D8614016DE8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{25159FD2-BAFB-44FA-A08A-40EFAA6874EE}"/>
   </bookViews>
@@ -7215,6 +7215,18 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A206:F206"/>
+    <mergeCell ref="A210:F210"/>
+    <mergeCell ref="A214:F214"/>
+    <mergeCell ref="A227:F227"/>
+    <mergeCell ref="A222:F222"/>
+    <mergeCell ref="A218:F218"/>
+    <mergeCell ref="A146:F146"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A43:F43"/>
+    <mergeCell ref="A104:F104"/>
+    <mergeCell ref="A121:F121"/>
     <mergeCell ref="A194:F194"/>
     <mergeCell ref="A202:F202"/>
     <mergeCell ref="A154:F154"/>
@@ -7222,18 +7234,6 @@
     <mergeCell ref="A170:F170"/>
     <mergeCell ref="A178:F178"/>
     <mergeCell ref="A186:F186"/>
-    <mergeCell ref="A146:F146"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A43:F43"/>
-    <mergeCell ref="A104:F104"/>
-    <mergeCell ref="A121:F121"/>
-    <mergeCell ref="A206:F206"/>
-    <mergeCell ref="A210:F210"/>
-    <mergeCell ref="A214:F214"/>
-    <mergeCell ref="A227:F227"/>
-    <mergeCell ref="A222:F222"/>
-    <mergeCell ref="A218:F218"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7246,10 +7246,10 @@
   <dimension ref="A1:M208"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E68" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M49" sqref="M49"/>
+      <selection pane="bottomRight" activeCell="M86" sqref="M86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Prepared automatic control for all stages type
</commit_message>
<xml_diff>
--- a/DOCs/Modbus.Table.v5.xlsx
+++ b/DOCs/Modbus.Table.v5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tranings\NTCC.NET\DOCs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD476EA-3075-4DB7-AC95-D8614016DE8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D18BEE1F-9C60-4E31-B133-0D47B07F0E10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{25159FD2-BAFB-44FA-A08A-40EFAA6874EE}"/>
   </bookViews>
@@ -7246,10 +7246,10 @@
   <dimension ref="A1:M208"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E68" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E73" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M86" sqref="M86"/>
+      <selection pane="bottomRight" activeCell="M84" sqref="M84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>